<commit_message>
Insertion en bd complète
</commit_message>
<xml_diff>
--- a/data/out/Country_code.xlsx
+++ b/data/out/Country_code.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,334 +472,370 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Erythrée</t>
+          <t>Egypte</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ER</t>
+          <t>EG</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ethiopie</t>
+          <t>Erythrée</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ET</t>
+          <t>ER</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Madagascar</t>
+          <t>Ethiopie</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>ET</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Maroc</t>
+          <t>Madagascar</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MA</t>
+          <t>MG</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Maurice</t>
+          <t>Maroc</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MU</t>
+          <t>MA</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Réunion</t>
+          <t>Maurice</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>RE</t>
+          <t>MU</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Tunisie</t>
+          <t>Réunion</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>RE</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Togo</t>
+          <t>Tunisie</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>TN</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Tchad</t>
+          <t>Togo</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TD</t>
+          <t>TG</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Sénégal</t>
+          <t>Tchad</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SN</t>
+          <t>TD</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Mali</t>
+          <t>Sénégal</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ML</t>
+          <t>SN</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Ghana</t>
+          <t>Mali</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>GH</t>
+          <t>ML</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Guinée</t>
+          <t>Ghana</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>GN</t>
+          <t>GH</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Botswana</t>
+          <t>Centafrique</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BW</t>
+          <t>CE</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Afrique du Sud</t>
+          <t>Côte Ivoire</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ZA</t>
+          <t>CI</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Eswatini</t>
+          <t>Guinée</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SZ</t>
+          <t>GN</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Malawi</t>
+          <t>Botswana</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MW</t>
+          <t>BW</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Angola</t>
+          <t>Afrique du Sud</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>AO</t>
+          <t>ZA</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Mozambique</t>
+          <t>Eswatini</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>MZ</t>
+          <t>SZ</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Namibie</t>
+          <t>Malawi</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>MW</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Zimbabwe</t>
+          <t>Angola</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ZW</t>
+          <t>AO</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Zambie</t>
+          <t>Mozambique</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ZM</t>
+          <t>MZ</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Cameroun</t>
+          <t>Namibie</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>CM</t>
+          <t>NA</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>RDC</t>
+          <t>Zimbabwe</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>ZW</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Gabon</t>
+          <t>Zambie</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>GA</t>
+          <t>ZM</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Kenya</t>
+          <t>Cameroun</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>KE</t>
+          <t>CM</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Uganda</t>
+          <t>RDC</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>UG</t>
+          <t>CD</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>Gabon</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Kenya</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>KE</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Uganda</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>UG</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
           <t>Tanzania</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B34" t="inlineStr">
         <is>
           <t>TZ</t>
         </is>

</xml_diff>